<commit_message>
First working version.  Need to finish off user-defined fields
</commit_message>
<xml_diff>
--- a/samples/Arrearage Template.xlsx
+++ b/samples/Arrearage Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="235" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="4" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="datasheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="136">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -144,13 +144,22 @@
     <t>date</t>
   </si>
   <si>
-    <t>creator_1</t>
-  </si>
-  <si>
-    <t>creator_2</t>
-  </si>
-  <si>
-    <t>creator_3</t>
+    <t>creator_1_primary_name</t>
+  </si>
+  <si>
+    <t>creator_1_rest_of_name</t>
+  </si>
+  <si>
+    <t>creator_2_primary_name</t>
+  </si>
+  <si>
+    <t>creator_2_rest_of_name</t>
+  </si>
+  <si>
+    <t>creator_3_primary_name</t>
+  </si>
+  <si>
+    <t>creator_3_rest_of_name</t>
   </si>
   <si>
     <t>linked_corporate_entity_agent</t>
@@ -191,8 +200,7 @@
     <t>Level of description</t>
   </si>
   <si>
-    <t>Previous Location
-</t>
+    <t>Previous Location</t>
   </si>
   <si>
     <t>Room</t>
@@ -213,13 +221,22 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Creator 1</t>
-  </si>
-  <si>
-    <t>Creator 2</t>
-  </si>
-  <si>
-    <t>Creator 3</t>
+    <t>Creator 1 Primary Name</t>
+  </si>
+  <si>
+    <t>Creator 1 Rest Of Name</t>
+  </si>
+  <si>
+    <t>Creator 2 Primary Name</t>
+  </si>
+  <si>
+    <t>Creator 2 Rest Of Name</t>
+  </si>
+  <si>
+    <t>Creator 3 Primary Name</t>
+  </si>
+  <si>
+    <t>Creator 3 Rest Of Name</t>
   </si>
   <si>
     <t>Corporate Creator</t>
@@ -295,7 +312,10 @@
     <t>ca. 1870-ca. 1897</t>
   </si>
   <si>
-    <t>Charles Bayliss</t>
+    <t>Bayliss</t>
+  </si>
+  <si>
+    <t>Charles</t>
   </si>
   <si>
     <t>Bayliss Collection</t>
@@ -316,7 +336,7 @@
     <t>Collection of photographs of the Snowy Mountains</t>
   </si>
   <si>
-    <t>Charles D'Arcy</t>
+    <t>D'Arcy</t>
   </si>
   <si>
     <t>PIC/12351/1</t>
@@ -400,10 +420,13 @@
     <t>Blundell's Cottage, Canberra</t>
   </si>
   <si>
-    <t>Alex Hood</t>
-  </si>
-  <si>
-    <t>Annette Hood</t>
+    <t>Hood</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Annette</t>
   </si>
   <si>
     <t>Hold pending rights negotiation.</t>
@@ -552,7 +575,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
@@ -641,13 +664,6 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
   </cellXfs>
@@ -727,40 +743,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:X14"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="B3" xSplit="1" ySplit="2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="B1" activeCellId="0" pane="topRight" sqref="B1"/>
-      <selection activeCell="A3" activeCellId="0" pane="bottomLeft" sqref="A3"/>
-      <selection activeCell="B24" activeCellId="0" pane="bottomRight" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.6274509803922"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="14.2"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="10.6117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="16.3490196078431"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.3254901960784"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8980392156863"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="7.45882352941177"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="5.45098039215686"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="6.74117647058824"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="9.18039215686274"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="26.1098039215686"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="7.02745098039216"/>
-    <col collapsed="false" hidden="false" max="16" min="14" style="2" width="12.6196078431373"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="9.32156862745098"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="2" width="12.0470588235294"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="8.60392156862745"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="30.1254901960784"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="16.2078431372549"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="9.18039215686274"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="13.6235294117647"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="31.9882352941176"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="2" width="9.18039215686274"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.6862745098039"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="14.2549019607843"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.2313725490196"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="10.6549019607843"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="16.4156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.3686274509804"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.9411764705882"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="7.48627450980392"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="6.76862745098039"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="9.22352941176471"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="26.2156862745098"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="7.05490196078431"/>
+    <col collapsed="false" hidden="false" max="20" min="14" style="2" width="12.6705882352941"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="9.35686274509804"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="2" width="12.0980392156863"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="30.2549019607843"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="16.2705882352941"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="2" width="9.22352941176471"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="2" width="13.6823529411765"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="2" width="32.1176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="2" width="9.22352941176471"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="51" outlineLevel="0" r="1">
@@ -797,37 +809,41 @@
       <c r="M1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="N1" s="5"/>
       <c r="O1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="P1" s="5"/>
       <c r="Q1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>8</v>
       </c>
     </row>
@@ -865,37 +881,41 @@
       <c r="M2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="N2" s="10"/>
       <c r="O2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="V2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="W2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="X2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="Y2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="Z2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="AA2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="AB2" s="13" t="s">
         <v>27</v>
       </c>
     </row>
@@ -924,6 +944,10 @@
       <c r="V3" s="15"/>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="15"/>
+      <c r="AB3" s="15"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="41.75" outlineLevel="0" r="4" s="22">
       <c r="A4" s="18" t="s">
@@ -965,129 +989,149 @@
       <c r="M4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="19"/>
+      <c r="O4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="P4" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="19" t="s">
+      <c r="Q4" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="19" t="s">
+      <c r="R4" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="R4" s="19" t="s">
+      <c r="S4" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="S4" s="19" t="s">
+      <c r="T4" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="T4" s="19" t="s">
+      <c r="U4" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="U4" s="19" t="s">
+      <c r="V4" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="19" t="s">
+      <c r="W4" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="W4" s="19" t="s">
+      <c r="X4" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="X4" s="19" t="s">
+      <c r="Y4" s="19" t="s">
         <v>51</v>
+      </c>
+      <c r="Z4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA4" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB4" s="19" t="s">
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="46.25" outlineLevel="0" r="5" s="25">
       <c r="A5" s="1"/>
       <c r="B5" s="23" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="L5" s="23" t="s">
         <v>17</v>
       </c>
       <c r="M5" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="N5" s="23" t="s">
-        <v>63</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="N5" s="23"/>
       <c r="O5" s="23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="P5" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q5" s="23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R5" s="23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S5" s="23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="T5" s="23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="U5" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="V5" s="23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="W5" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="X5" s="23" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="Y5" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z5" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA5" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB5" s="23" t="s">
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="6">
       <c r="B6" s="26" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="26" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="15" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="I6" s="15" t="n">
         <v>4</v>
@@ -1099,56 +1143,60 @@
         <v>1</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="M6" s="26" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="N6" s="26"/>
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
       <c r="Q6" s="26"/>
-      <c r="R6" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="S6" s="26" t="n">
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="W6" s="26" t="n">
         <v>16745</v>
       </c>
-      <c r="T6" s="26" t="n">
+      <c r="X6" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="U6" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="V6" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="W6" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="X6" s="26" t="s">
-        <v>84</v>
+      <c r="Y6" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z6" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA6" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB6" s="26" t="s">
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="7">
       <c r="B7" s="26" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="26" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="I7" s="15" t="n">
         <v>1</v>
@@ -1158,394 +1206,442 @@
       </c>
       <c r="K7" s="15"/>
       <c r="L7" s="15" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="N7" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
+        <v>95</v>
+      </c>
+      <c r="N7" s="15"/>
+      <c r="O7" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="P7" s="26" t="s">
+        <v>97</v>
+      </c>
       <c r="Q7" s="26"/>
-      <c r="R7" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="R7" s="26"/>
       <c r="S7" s="26"/>
-      <c r="T7" s="26" t="n">
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="W7" s="26"/>
+      <c r="X7" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="U7" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="V7" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="W7" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="X7" s="26"/>
+      <c r="Y7" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z7" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA7" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB7" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="8">
       <c r="B8" s="26"/>
       <c r="C8" s="26" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
+        <v>81</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="15" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="M8" s="26" t="n">
         <v>1935</v>
       </c>
-      <c r="N8" s="26" t="s">
+      <c r="N8" s="26"/>
+      <c r="O8" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="P8" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
       <c r="Q8" s="26"/>
       <c r="R8" s="26"/>
       <c r="S8" s="26"/>
-      <c r="T8" s="26" t="n">
-        <v>30</v>
-      </c>
+      <c r="T8" s="26"/>
       <c r="U8" s="26"/>
       <c r="V8" s="26"/>
       <c r="W8" s="26"/>
-      <c r="X8" s="26"/>
+      <c r="X8" s="26" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="26"/>
+      <c r="AA8" s="26"/>
+      <c r="AB8" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="9">
       <c r="B9" s="26" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D9" s="27" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="F9" s="26"/>
-      <c r="G9" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="H9" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="I9" s="29" t="n">
+      <c r="G9" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="J9" s="29" t="n">
+      <c r="J9" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="K9" s="29"/>
+      <c r="K9" s="15"/>
       <c r="L9" s="15" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="M9" s="26" t="n">
         <v>1935</v>
       </c>
-      <c r="N9" s="26" t="s">
+      <c r="N9" s="26"/>
+      <c r="O9" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="P9" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
       <c r="Q9" s="26"/>
       <c r="R9" s="26"/>
       <c r="S9" s="26"/>
-      <c r="T9" s="26" t="n">
+      <c r="T9" s="26"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="U9" s="26" t="s">
+      <c r="Y9" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z9" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA9" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="V9" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="W9" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="X9" s="26"/>
+      <c r="AB9" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="B10" s="26" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D10" s="27" t="n">
         <v>2</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="F10" s="26"/>
-      <c r="G10" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="H10" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="I10" s="29" t="n">
+      <c r="G10" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="J10" s="29" t="n">
+      <c r="J10" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="K10" s="29"/>
+      <c r="K10" s="15"/>
       <c r="L10" s="26" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="M10" s="26" t="n">
         <v>1935</v>
       </c>
-      <c r="N10" s="26" t="s">
+      <c r="N10" s="26"/>
+      <c r="O10" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="P10" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
       <c r="Q10" s="26"/>
       <c r="R10" s="26"/>
       <c r="S10" s="26"/>
-      <c r="T10" s="26" t="n">
+      <c r="T10" s="26"/>
+      <c r="U10" s="26"/>
+      <c r="V10" s="26"/>
+      <c r="W10" s="26"/>
+      <c r="X10" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="U10" s="26" t="s">
+      <c r="Y10" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z10" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA10" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="V10" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="W10" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="X10" s="26"/>
+      <c r="AB10" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="11">
       <c r="B11" s="26" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="F11" s="26"/>
-      <c r="G11" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="H11" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" s="29" t="n">
+      <c r="G11" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="J11" s="29" t="n">
+      <c r="J11" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="K11" s="29"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="26" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="M11" s="26" t="n">
         <v>1935</v>
       </c>
-      <c r="N11" s="26" t="s">
+      <c r="N11" s="26"/>
+      <c r="O11" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="P11" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
       <c r="Q11" s="26"/>
       <c r="R11" s="26"/>
       <c r="S11" s="26"/>
-      <c r="T11" s="26" t="n">
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="26"/>
+      <c r="W11" s="26"/>
+      <c r="X11" s="26" t="n">
         <v>27</v>
       </c>
-      <c r="U11" s="26" t="s">
+      <c r="Y11" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z11" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="V11" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="W11" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="X11" s="26"/>
+      <c r="AA11" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB11" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="B12" s="26" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="F12" s="26"/>
-      <c r="G12" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="H12" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="I12" s="29" t="n">
+      <c r="G12" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="J12" s="29" t="n">
+      <c r="J12" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="K12" s="29"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="26" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="M12" s="26" t="n">
         <v>1935</v>
       </c>
-      <c r="N12" s="26" t="s">
+      <c r="N12" s="26"/>
+      <c r="O12" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="P12" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
       <c r="Q12" s="26"/>
       <c r="R12" s="26"/>
       <c r="S12" s="26"/>
-      <c r="T12" s="26" t="n">
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="U12" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="V12" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="W12" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="X12" s="26"/>
+      <c r="Y12" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z12" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA12" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB12" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="13">
       <c r="B13" s="26" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="29" t="s">
-        <v>115</v>
+        <v>81</v>
+      </c>
+      <c r="F13" s="26"/>
+      <c r="G13" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="26" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="M13" s="26" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="N13" s="26"/>
       <c r="O13" s="26"/>
       <c r="P13" s="26"/>
-      <c r="Q13" s="26" t="s">
-        <v>119</v>
-      </c>
+      <c r="Q13" s="26"/>
       <c r="R13" s="26"/>
-      <c r="S13" s="26" t="n">
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="V13" s="26"/>
+      <c r="W13" s="26" t="n">
         <v>38762</v>
       </c>
-      <c r="T13" s="26" t="n">
+      <c r="X13" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="U13" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="V13" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="W13" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="X13" s="26"/>
+      <c r="Y13" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z13" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA13" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB13" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="14">
       <c r="B14" s="26" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29" t="s">
-        <v>115</v>
+        <v>81</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
       <c r="L14" s="15" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="M14" s="26" t="n">
         <v>1975</v>
       </c>
-      <c r="N14" s="26" t="s">
-        <v>125</v>
-      </c>
+      <c r="N14" s="26"/>
       <c r="O14" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
+        <v>132</v>
+      </c>
+      <c r="P14" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q14" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="R14" s="26" t="s">
+        <v>134</v>
+      </c>
       <c r="S14" s="26"/>
-      <c r="T14" s="26" t="n">
+      <c r="T14" s="26"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="U14" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="V14" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="W14" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="X14" s="26" t="s">
+      <c r="Y14" s="26" t="s">
         <v>127</v>
+      </c>
+      <c r="Z14" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA14" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB14" s="26" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1553,23 +1649,19 @@
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="G2:J2"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="W6:W14" type="list">
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="AA6:AA14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E6" type="list">
-      <formula1>"Collection,Set,Item"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E7:E14" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E6:E14" type="list">
       <formula1>"Collection,Set,Item"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.159722222222222" top="0.479861111111111" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="0" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="77" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="0" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1589,28 +1681,28 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5960784313726"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.18039215686274"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.678431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.22352941176471"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
-      <c r="A1" s="30" t="s">
-        <v>55</v>
+      <c r="A1" s="28" t="s">
+        <v>58</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="A2" s="26" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
       <c r="A3" s="26" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="A4" s="26" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incorporate feedback from Megan
</commit_message>
<xml_diff>
--- a/samples/Arrearage Template.xlsx
+++ b/samples/Arrearage Template.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="176">
   <si>
     <t>Description of change from original template</t>
   </si>
@@ -208,7 +208,13 @@
     <t>location_shelf</t>
   </si>
   <si>
+    <t>type_1</t>
+  </si>
+  <si>
     <t>indicator_1</t>
+  </si>
+  <si>
+    <t>type_2</t>
   </si>
   <si>
     <t>indicator_2</t>
@@ -286,8 +292,7 @@
     <t>Description Level</t>
   </si>
   <si>
-    <t>Previous Location
-</t>
+    <t>Previous Location</t>
   </si>
   <si>
     <t>Room / Stack</t>
@@ -302,7 +307,13 @@
     <t>Shelf</t>
   </si>
   <si>
+    <t>Parent Box Type</t>
+  </si>
+  <si>
     <t>Parent Box</t>
+  </si>
+  <si>
+    <t>Child Box Type</t>
   </si>
   <si>
     <t>Child Box</t>
@@ -382,6 +393,9 @@
     <t>A4</t>
   </si>
   <si>
+    <t>box</t>
+  </si>
+  <si>
     <t>Dame Mary Hughes and two ladies having a picnic</t>
   </si>
   <si>
@@ -548,10 +562,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="@" numFmtId="165"/>
-    <numFmt formatCode="@" numFmtId="166"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -729,7 +742,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
@@ -793,7 +806,7 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="7" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -832,13 +845,6 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="8" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="false"/>
@@ -846,13 +852,6 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="8" fillId="0" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="8" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="9" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
@@ -935,36 +934,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF14"/>
+  <dimension ref="A1:AH14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="Y2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="AD4" activeCellId="0" pane="topLeft" sqref="AD4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.8039215686274"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.9450980392157"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.6666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.5137254901961"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.6666666666667"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.0470588235294"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.6666666666667"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.8470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="22.9450980392157"/>
-    <col collapsed="false" hidden="false" max="20" min="13" style="1" width="22.6666666666667"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="22.9450980392157"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.6666666666667"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="20.0862745098039"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="22.6666666666667"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="9.18039215686274"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="22.0941176470588"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="19.9333333333333"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="22.9450980392157"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="22.6666666666667"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="22.2352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="9.18039215686274"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.6078431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.9019607843137"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.0392156862745"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.7607843137255"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.6039215686275"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.7607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.0980392156863"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.7607843137255"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.8980392156863"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="1" width="23.0392156862745"/>
+    <col collapsed="false" hidden="false" max="22" min="15" style="1" width="22.7607843137255"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="23.0392156862745"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="22.7607843137255"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="20.1725490196078"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="22.7607843137255"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="9.22352941176471"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="22.1882352941176"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="20.0196078431373"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="23.0392156862745"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="22.7607843137255"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="22.3294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="9.22352941176471"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="102.2" outlineLevel="0" r="1" s="6">
@@ -998,58 +997,60 @@
       <c r="J1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R1" s="3"/>
       <c r="S1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1078,22 +1079,20 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
-      <c r="K2" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="K2" s="10"/>
       <c r="L2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="8"/>
+      <c r="N2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="P2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="8"/>
       <c r="Q2" s="8" t="s">
         <v>26</v>
       </c>
@@ -1101,37 +1100,41 @@
       <c r="S2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="8"/>
+      <c r="U2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="V2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="X2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="Y2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="Z2" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="Y2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z2" s="11" t="s">
-        <v>31</v>
       </c>
       <c r="AA2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AB2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AC2" s="8" t="s">
+      <c r="AC2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AD2" s="12" t="s">
+      <c r="AF2" s="12" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1160,18 +1163,16 @@
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="16"/>
+      <c r="L3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="M3" s="17"/>
+      <c r="N3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="O3" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14" t="s">
-        <v>41</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14" t="s">
@@ -1181,37 +1182,41 @@
       <c r="S3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="14"/>
+      <c r="U3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="V3" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="U3" s="14" t="s">
+      <c r="W3" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="X3" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="W3" s="17" t="s">
+      <c r="Y3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="X3" s="17" t="s">
+      <c r="Z3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="Y3" s="17" t="s">
+      <c r="AA3" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="Z3" s="17" t="s">
+      <c r="AB3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="AA3" s="17" t="s">
+      <c r="AC3" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="AB3" s="14" t="s">
+      <c r="AD3" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="AC3" s="17" t="s">
+      <c r="AE3" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="AD3" s="18" t="s">
+      <c r="AF3" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1306,117 +1311,129 @@
       <c r="AD4" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="AE4" s="20"/>
-      <c r="AF4" s="20"/>
+      <c r="AE4" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF4" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG4" s="20"/>
+      <c r="AH4" s="20"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="57.45" outlineLevel="0" r="5">
       <c r="A5" s="24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K5" s="25" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L5" s="25" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M5" s="25" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N5" s="25" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="O5" s="25" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="P5" s="25" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="Q5" s="25" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="R5" s="25" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="S5" s="25" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="T5" s="25" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="U5" s="25" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="V5" s="25" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="W5" s="25" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="X5" s="25" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="Y5" s="25" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="Z5" s="25" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AA5" s="25" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AB5" s="25" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="AC5" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="AD5" s="27" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="AD5" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE5" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF5" s="27" t="s">
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="6">
       <c r="A6" s="24"/>
       <c r="B6" s="28" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C6" s="28"/>
       <c r="D6" s="29"/>
       <c r="E6" s="28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="30" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="I6" s="30" t="n">
         <v>4</v>
@@ -1424,69 +1441,73 @@
       <c r="J6" s="30" t="n">
         <v>6</v>
       </c>
-      <c r="K6" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30" t="s">
-        <v>117</v>
-      </c>
+      <c r="K6" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="L6" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="30"/>
       <c r="N6" s="30"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
+      <c r="O6" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="P6" s="30"/>
       <c r="Q6" s="28"/>
       <c r="R6" s="28"/>
       <c r="S6" s="28"/>
       <c r="T6" s="28"/>
-      <c r="U6" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="V6" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="W6" s="28" t="n">
+      <c r="U6" s="28"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="X6" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y6" s="28" t="n">
         <v>16745</v>
       </c>
-      <c r="X6" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA6" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="AB6" s="30" t="s">
-        <v>122</v>
+      <c r="Z6" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="28" t="s">
+        <v>125</v>
       </c>
       <c r="AC6" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD6" s="31" t="s">
-        <v>124</v>
+        <v>126</v>
+      </c>
+      <c r="AD6" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE6" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF6" s="31" t="s">
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="7">
       <c r="A7" s="24"/>
       <c r="B7" s="28" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="29"/>
       <c r="E7" s="28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="I7" s="30" t="n">
         <v>1</v>
@@ -1494,499 +1515,531 @@
       <c r="J7" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="K7" s="30" t="n">
-        <v>1</v>
+      <c r="K7" s="30" t="s">
+        <v>121</v>
       </c>
       <c r="L7" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30" t="n">
         <v>24</v>
       </c>
-      <c r="M7" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="N7" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="O7" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
+      <c r="O7" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="P7" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q7" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="R7" s="28"/>
       <c r="S7" s="28"/>
       <c r="T7" s="28"/>
-      <c r="U7" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="V7" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="W7" s="28" t="n">
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="X7" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y7" s="28" t="n">
         <v>29842</v>
       </c>
-      <c r="X7" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA7" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="AB7" s="30" t="s">
-        <v>134</v>
+      <c r="Z7" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="28" t="s">
+        <v>125</v>
       </c>
       <c r="AC7" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD7" s="31"/>
+        <v>138</v>
+      </c>
+      <c r="AD7" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE7" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF7" s="31"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="8">
       <c r="A8" s="24"/>
       <c r="B8" s="28" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="29"/>
       <c r="E8" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="N8" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="O8" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
+        <v>142</v>
+      </c>
+      <c r="F8" s="28"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="P8" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q8" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="R8" s="28"/>
       <c r="S8" s="28"/>
       <c r="T8" s="28"/>
-      <c r="U8" s="28" t="n">
-        <v>1935</v>
-      </c>
+      <c r="U8" s="28"/>
       <c r="V8" s="28"/>
       <c r="W8" s="28" t="n">
+        <v>1935</v>
+      </c>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="28" t="n">
         <v>288744</v>
       </c>
-      <c r="X8" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="28" t="n">
+      <c r="Z8" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="Z8" s="28" t="s">
+      <c r="AB8" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC8" s="28"/>
+      <c r="AD8" s="28"/>
+      <c r="AE8" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="AA8" s="28"/>
-      <c r="AB8" s="28"/>
-      <c r="AC8" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD8" s="31"/>
+      <c r="AF8" s="31"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="9">
       <c r="A9" s="24"/>
       <c r="B9" s="28" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="F9" s="28"/>
-      <c r="G9" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="H9" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="I9" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="33" t="n">
+      <c r="G9" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="I9" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="30" t="s">
+      <c r="K9" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="P9" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="N9" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="O9" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
+      <c r="Q9" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="R9" s="28"/>
       <c r="S9" s="28"/>
       <c r="T9" s="28"/>
-      <c r="U9" s="28" t="n">
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28" t="n">
         <v>1935</v>
       </c>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
-      <c r="X9" s="28" t="n">
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="Y9" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA9" s="28" t="s">
-        <v>145</v>
+      <c r="AA9" s="28" t="n">
+        <v>1</v>
       </c>
       <c r="AB9" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="AC9" s="28"/>
-      <c r="AD9" s="31"/>
+        <v>125</v>
+      </c>
+      <c r="AC9" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD9" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE9" s="28"/>
+      <c r="AF9" s="31"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="10">
       <c r="A10" s="24"/>
       <c r="B10" s="28" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="F10" s="28"/>
-      <c r="G10" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="H10" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="I10" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="33" t="n">
+      <c r="G10" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="I10" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="N10" s="30" t="s">
-        <v>139</v>
-      </c>
+      <c r="K10" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
       <c r="O10" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
+        <v>153</v>
+      </c>
+      <c r="P10" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q10" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="R10" s="28"/>
       <c r="S10" s="28"/>
       <c r="T10" s="28"/>
-      <c r="U10" s="28" t="n">
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28" t="n">
         <v>1935</v>
       </c>
-      <c r="V10" s="28"/>
-      <c r="W10" s="28"/>
-      <c r="X10" s="28" t="n">
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="Y10" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA10" s="28" t="s">
-        <v>145</v>
+      <c r="AA10" s="28" t="n">
+        <v>1</v>
       </c>
       <c r="AB10" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="AC10" s="28"/>
-      <c r="AD10" s="31"/>
+        <v>125</v>
+      </c>
+      <c r="AC10" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD10" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE10" s="28"/>
+      <c r="AF10" s="31"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="11">
       <c r="A11" s="24"/>
       <c r="B11" s="28" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F11" s="28"/>
-      <c r="G11" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="I11" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="33" t="n">
+      <c r="G11" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="I11" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="N11" s="30" t="s">
-        <v>139</v>
-      </c>
+      <c r="K11" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
       <c r="O11" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
+        <v>156</v>
+      </c>
+      <c r="P11" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q11" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="R11" s="28"/>
       <c r="S11" s="28"/>
       <c r="T11" s="28"/>
-      <c r="U11" s="28" t="n">
+      <c r="U11" s="28"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="28" t="n">
         <v>1935</v>
       </c>
-      <c r="V11" s="28"/>
-      <c r="W11" s="28"/>
-      <c r="X11" s="28" t="n">
+      <c r="X11" s="28"/>
+      <c r="Y11" s="28"/>
+      <c r="Z11" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="Y11" s="28" t="n">
+      <c r="AA11" s="28" t="n">
         <v>27</v>
       </c>
-      <c r="Z11" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="AA11" s="28" t="s">
-        <v>152</v>
-      </c>
       <c r="AB11" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="AC11" s="28"/>
-      <c r="AD11" s="31"/>
+        <v>145</v>
+      </c>
+      <c r="AC11" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="AD11" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE11" s="28"/>
+      <c r="AF11" s="31"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
       <c r="A12" s="24"/>
       <c r="B12" s="28" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="F12" s="28"/>
-      <c r="G12" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="H12" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="I12" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="33" t="n">
+      <c r="G12" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="N12" s="30" t="s">
-        <v>139</v>
-      </c>
+      <c r="K12" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
       <c r="O12" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
+        <v>159</v>
+      </c>
+      <c r="P12" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q12" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="R12" s="28"/>
       <c r="S12" s="28"/>
       <c r="T12" s="28"/>
-      <c r="U12" s="28" t="n">
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="28" t="n">
         <v>1935</v>
       </c>
-      <c r="V12" s="28"/>
-      <c r="W12" s="28"/>
-      <c r="X12" s="28" t="n">
+      <c r="X12" s="28"/>
+      <c r="Y12" s="28"/>
+      <c r="Z12" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="Y12" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA12" s="28" t="s">
-        <v>155</v>
+      <c r="AA12" s="28" t="n">
+        <v>1</v>
       </c>
       <c r="AB12" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="AC12" s="28"/>
-      <c r="AD12" s="31"/>
+        <v>125</v>
+      </c>
+      <c r="AC12" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AD12" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE12" s="28"/>
+      <c r="AF12" s="31"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
       <c r="A13" s="24"/>
       <c r="B13" s="28" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="29"/>
       <c r="E13" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33" t="s">
-        <v>157</v>
+        <v>118</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="30" t="s">
+        <v>162</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I13" s="30"/>
       <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
+      <c r="K13" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="L13" s="30"/>
-      <c r="M13" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="28" t="s">
+        <v>164</v>
+      </c>
       <c r="P13" s="28"/>
       <c r="Q13" s="28"/>
       <c r="R13" s="28"/>
       <c r="S13" s="28"/>
-      <c r="T13" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="U13" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="V13" s="28"/>
-      <c r="W13" s="28" t="n">
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="W13" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="28" t="n">
         <v>38762</v>
       </c>
-      <c r="X13" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA13" s="28" t="s">
-        <v>162</v>
+      <c r="Z13" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="28" t="n">
+        <v>1</v>
       </c>
       <c r="AB13" s="28" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="AC13" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD13" s="31"/>
+        <v>167</v>
+      </c>
+      <c r="AD13" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="AE13" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF13" s="31"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
       <c r="A14" s="24"/>
-      <c r="B14" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37" t="s">
-        <v>157</v>
+      <c r="B14" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="14" t="s">
+        <v>162</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
+      <c r="K14" s="14" t="s">
+        <v>121</v>
+      </c>
       <c r="L14" s="14"/>
-      <c r="M14" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="N14" s="14" t="s">
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q14" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="R14" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="S14" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="32" t="n">
+        <v>1975</v>
+      </c>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="32" t="n">
+        <v>887322</v>
+      </c>
+      <c r="Z14" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC14" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="O14" s="34" t="s">
+      <c r="AD14" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="P14" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q14" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="R14" s="34"/>
-      <c r="S14" s="34"/>
-      <c r="T14" s="34"/>
-      <c r="U14" s="34" t="n">
-        <v>1975</v>
-      </c>
-      <c r="V14" s="34"/>
-      <c r="W14" s="34" t="n">
-        <v>887322</v>
-      </c>
-      <c r="X14" s="34" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="34" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z14" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA14" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="AB14" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="AC14" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD14" s="38" t="s">
-        <v>170</v>
+      <c r="AE14" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF14" s="34" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2017,7 +2070,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2042,7 +2095,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>